<commit_message>
ajouts photos et textes for real
</commit_message>
<xml_diff>
--- a/Remises/Remise 2/PlanTest.xlsx
+++ b/Remises/Remise 2/PlanTest.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles-Olivier\Documents\Ulaval\Hiver 2016\Remises\Remise 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaetan\Documents\GitHub\design3\Remises\Remise 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12624"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -658,25 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -745,6 +727,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,7 +764,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1028,22 +1028,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.6328125" customWidth="1"/>
-    <col min="2" max="2" width="67.54296875" customWidth="1"/>
-    <col min="3" max="3" width="52.6328125" customWidth="1"/>
-    <col min="4" max="4" width="27.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.453125" customWidth="1"/>
+    <col min="1" max="1" width="66.6640625" customWidth="1"/>
+    <col min="2" max="2" width="67.5546875" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.44140625" customWidth="1"/>
     <col min="7" max="7" width="92" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1066,699 +1066,699 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
-    </row>
-    <row r="7" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="E7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="16" t="s">
+      <c r="E8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="16" t="s">
+      <c r="E9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-    </row>
-    <row r="12" spans="1:7" ht="38" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+    <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="26" t="s">
+      <c r="E12" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="38" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="27" t="s">
+      <c r="E13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="19" t="s">
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="E14" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="27" t="s">
+      <c r="E14" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="25" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="19" t="s">
+    <row r="15" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A15" s="32"/>
+      <c r="B15" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="E15" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="16" t="s">
+      <c r="E15" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="35" t="s">
+    <row r="16" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="22" t="s">
+      <c r="E16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="30" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
-    </row>
-    <row r="18" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="17" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="16" t="s">
+      <c r="E18" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="12" t="s">
+    <row r="19" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="E19" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="16" t="s">
+      <c r="E19" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="12" t="s">
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="16" t="s">
+      <c r="E20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
-    </row>
-    <row r="22" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="21" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="16" t="s">
+      <c r="E22" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="12" t="s">
+    <row r="23" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="35"/>
+      <c r="B23" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="16" t="s">
+      <c r="E23" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12" t="s">
+    <row r="24" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="36"/>
+      <c r="B24" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="32" t="s">
+      <c r="E24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="23"/>
-    </row>
-    <row r="26" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="12" t="s">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="12" t="s">
+    <row r="28" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
+      <c r="B28" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="16" t="s">
+      <c r="E28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="12" t="s">
+    <row r="29" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
+      <c r="B29" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="G29" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="12" t="s">
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
-    </row>
-    <row r="32" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="28">
         <v>0.95</v>
       </c>
-      <c r="E32" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="16" t="s">
+      <c r="E32" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="G32" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="12" t="s">
+    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="G33" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="12" t="s">
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
+      <c r="B34" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D34" s="28">
         <v>0.95</v>
       </c>
-      <c r="E34" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="16" t="s">
+      <c r="E34" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G34" s="17" t="s">
+      <c r="G34" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="12" t="s">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E35" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="16" t="s">
+      <c r="E35" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="G35" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="12" t="s">
+    <row r="36" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+      <c r="B36" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="34">
+      <c r="D36" s="28">
         <v>0.98</v>
       </c>
-      <c r="E36" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="16" t="s">
+      <c r="E36" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G36" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
   </sheetData>

</xml_diff>